<commit_message>
Baseline Models ELM, other traditional
added ELM, Naive Bayes, Decision Tree, Random Forest, knn
</commit_message>
<xml_diff>
--- a/results/results_overview.xlsx
+++ b/results/results_overview.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kim-Carolin\Documents\GitHub\automatic_speech_emotion_recognition\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB550639-0B54-4F02-83C6-9184AB4C054F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1002C6F1-7D57-4F4F-A7E0-9204D3CAB3F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14476" xr2:uid="{899EA679-B183-4A51-8A5C-67DA9C3D8107}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="142">
   <si>
     <t>SVM</t>
   </si>
@@ -556,6 +556,78 @@
   </si>
   <si>
     <t>63.67%</t>
+  </si>
+  <si>
+    <t>ELM</t>
+  </si>
+  <si>
+    <t>94.71%</t>
+  </si>
+  <si>
+    <t>66.80%</t>
+  </si>
+  <si>
+    <t>ufunc='sigm' (instead of tanh)</t>
+  </si>
+  <si>
+    <t>95.37%</t>
+  </si>
+  <si>
+    <t>66.57%</t>
+  </si>
+  <si>
+    <t>pairwise_metric='euclidean'</t>
+  </si>
+  <si>
+    <t>pairwise_metric='euclidean' (ufunc, density would anyways be ignored then, like rbf-kernel)</t>
+  </si>
+  <si>
+    <t>97.41%</t>
+  </si>
+  <si>
+    <t>73.09%</t>
+  </si>
+  <si>
+    <t>pairwise_metric='cosine'</t>
+  </si>
+  <si>
+    <t>91.73%</t>
+  </si>
+  <si>
+    <t>80.27%</t>
+  </si>
+  <si>
+    <t>worse train results but better generalization</t>
+  </si>
+  <si>
+    <t>94.75%</t>
+  </si>
+  <si>
+    <t>68.09%</t>
+  </si>
+  <si>
+    <t>features from paper - 16 selected (featurewiz)</t>
+  </si>
+  <si>
+    <t>63.92%</t>
+  </si>
+  <si>
+    <t>50.51%</t>
+  </si>
+  <si>
+    <t>91.86%</t>
+  </si>
+  <si>
+    <t>52.49%</t>
+  </si>
+  <si>
+    <t>worse after feature selection</t>
+  </si>
+  <si>
+    <t>81.65%</t>
+  </si>
+  <si>
+    <t>54.86%</t>
   </si>
 </sst>
 </file>
@@ -617,7 +689,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -677,11 +749,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -747,6 +828,24 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1063,11 +1162,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BC463B8-7CA3-421A-B5A9-34F975ADEC63}">
-  <dimension ref="A1:H35"/>
+  <dimension ref="A1:H44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F34" sqref="F34:G34"/>
+      <pane ySplit="1" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1079,7 +1178,8 @@
     <col min="5" max="5" width="34.1328125" style="4" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.19921875" style="5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.46484375" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.06640625" style="1"/>
+    <col min="8" max="8" width="35.796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.06640625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.45">
@@ -1813,7 +1913,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A33" s="20">
         <v>1</v>
       </c>
@@ -1836,7 +1936,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="34" spans="1:7" s="22" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:8" s="22" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A34" s="20">
         <v>1</v>
       </c>
@@ -1859,7 +1959,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="35" spans="1:7" s="22" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:8" s="22" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A35" s="20">
         <v>1</v>
       </c>
@@ -1881,6 +1981,210 @@
       <c r="G35" s="20" t="s">
         <v>117</v>
       </c>
+    </row>
+    <row r="36" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A36" s="5">
+        <v>2</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F36" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="G36" s="5" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A37" s="5">
+        <v>2</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="F37" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="G37" s="5" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A38" s="5">
+        <v>2</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="F38" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="G38" s="5" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A39" s="5">
+        <v>2</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="F39" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="G39" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A40" s="5">
+        <v>2</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E40" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F40" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="G40" s="5" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A41" s="5">
+        <v>2</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="E41" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="F41" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="G41" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A42" s="5">
+        <v>2</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="E42" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="F42" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="G42" s="5" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="28.9" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A43" s="25">
+        <v>2</v>
+      </c>
+      <c r="B43" s="26" t="s">
+        <v>134</v>
+      </c>
+      <c r="C43" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="D43" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="E43" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="F43" s="25" t="s">
+        <v>140</v>
+      </c>
+      <c r="G43" s="25" t="s">
+        <v>141</v>
+      </c>
+      <c r="H43" s="27"/>
+    </row>
+    <row r="44" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A44" s="23"/>
+      <c r="B44" s="28" t="s">
+        <v>84</v>
+      </c>
+      <c r="C44" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="D44" s="24"/>
+      <c r="E44" s="24"/>
+      <c r="F44" s="23"/>
+      <c r="G44" s="23"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
Experiments for MLPNN, GFFNN added
added adjusted architecture like in paper 1 to the neural nets
</commit_message>
<xml_diff>
--- a/results/results_overview.xlsx
+++ b/results/results_overview.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kim-Carolin\Documents\GitHub\automatic_speech_emotion_recognition\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16F2FD87-1CE5-4FF8-B8F4-F4D62B8D79E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CC6429B-E642-4EB5-99DA-BDA01862B1E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7860" yWindow="0" windowWidth="14723" windowHeight="14362" xr2:uid="{899EA679-B183-4A51-8A5C-67DA9C3D8107}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14476" activeTab="1" xr2:uid="{899EA679-B183-4A51-8A5C-67DA9C3D8107}"/>
   </bookViews>
   <sheets>
     <sheet name="TraditionalML" sheetId="1" r:id="rId1"/>
-    <sheet name="TraditionalML_enhanced_data" sheetId="3" r:id="rId2"/>
-    <sheet name="TraditionalML_female_male_dif" sheetId="2" r:id="rId3"/>
-    <sheet name="TraditionalML_top_features_only" sheetId="4" r:id="rId4"/>
+    <sheet name="TraditionalML_NNexperiments" sheetId="5" r:id="rId2"/>
+    <sheet name="TraditionalML_enhanced_data" sheetId="3" r:id="rId3"/>
+    <sheet name="TraditionalML_female_male_dif" sheetId="2" r:id="rId4"/>
+    <sheet name="TraditionalML_top_features_only" sheetId="4" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">TraditionalML!$A$1:$H$54</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">TraditionalML_female_male_dif!$A$1:$I$33</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">TraditionalML_female_male_dif!$A$1:$I$33</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="945" uniqueCount="345">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1065" uniqueCount="392">
   <si>
     <t>SVM</t>
   </si>
@@ -1280,6 +1281,147 @@
   </si>
   <si>
     <t>79.35%</t>
+  </si>
+  <si>
+    <t>Adam optimizer, Cross-entropy loss stayed the same for all models</t>
+  </si>
+  <si>
+    <t>MLP-FFNN - hidden 3</t>
+  </si>
+  <si>
+    <t>GFFNN - hidden 5</t>
+  </si>
+  <si>
+    <t>hidden_dims: 64-128-64</t>
+  </si>
+  <si>
+    <t>99.48%</t>
+  </si>
+  <si>
+    <t>82.81%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hidden_dims = [128, 64, 32, 64, 128]; skip only to hidden layer 3 </t>
+  </si>
+  <si>
+    <t>hidden_dims = [128, 64, 32, 64, 128]; skip only to hidden layer 4</t>
+  </si>
+  <si>
+    <t>hidden_dims = [128, 64, 32, 64, 128]; skip only to hidden layer 5</t>
+  </si>
+  <si>
+    <t>hidden_dims = [128, 64, 32, 64, 128]; skip only to hidden layer 2</t>
+  </si>
+  <si>
+    <t>hidden_dims = [128, 64, 32, 64, 128]; skip to all hidden layers (except first)</t>
+  </si>
+  <si>
+    <t>93.42%</t>
+  </si>
+  <si>
+    <t>74.83%</t>
+  </si>
+  <si>
+    <t>86.24%</t>
+  </si>
+  <si>
+    <t>hidden_dims = [32, 32, 32, 32, 32]; skip only to hidden layer 4</t>
+  </si>
+  <si>
+    <t>85.60%</t>
+  </si>
+  <si>
+    <t>85.48%</t>
+  </si>
+  <si>
+    <t>89.49%</t>
+  </si>
+  <si>
+    <t>79.83%</t>
+  </si>
+  <si>
+    <t>80.51%</t>
+  </si>
+  <si>
+    <t>hidden_dims = [64, 32, 16, 32, 64]; skip only to hidden layer 4</t>
+  </si>
+  <si>
+    <t>99.32%</t>
+  </si>
+  <si>
+    <t>87.95%</t>
+  </si>
+  <si>
+    <t>most important 97</t>
+  </si>
+  <si>
+    <t>hidden_dims = 64, 32, 64</t>
+  </si>
+  <si>
+    <t>99.61%</t>
+  </si>
+  <si>
+    <t>77.94%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">91.58% </t>
+  </si>
+  <si>
+    <t>74.36%</t>
+  </si>
+  <si>
+    <t>hidden_dims = [64, 32, 16, 32, 64] ; skip only to hidden layer 4</t>
+  </si>
+  <si>
+    <t>43.89%</t>
+  </si>
+  <si>
+    <t>41.96%</t>
+  </si>
+  <si>
+    <t>hidden_dims = 10, 10, 10</t>
+  </si>
+  <si>
+    <t>66.77%</t>
+  </si>
+  <si>
+    <t>59.52%</t>
+  </si>
+  <si>
+    <t>hidden_dims = 32, 64, 32</t>
+  </si>
+  <si>
+    <t>99.45%</t>
+  </si>
+  <si>
+    <t>70.65%</t>
+  </si>
+  <si>
+    <t>hidden_dims = [19, 19, 19, 19, 19]; skip only to hidden layer 4</t>
+  </si>
+  <si>
+    <t>37.07%</t>
+  </si>
+  <si>
+    <t>29.86%</t>
+  </si>
+  <si>
+    <t>93.30%</t>
+  </si>
+  <si>
+    <t>68.81%</t>
+  </si>
+  <si>
+    <t>PCA from all numerical features -&gt; 47 features</t>
+  </si>
+  <si>
+    <t>best model with PCA -&gt; results in exact same result</t>
+  </si>
+  <si>
+    <t>very bad with same PEs!</t>
+  </si>
+  <si>
+    <t>bad with same PEs!</t>
   </si>
 </sst>
 </file>
@@ -1667,29 +1809,29 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2007,9 +2149,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BC463B8-7CA3-421A-B5A9-34F975ADEC63}">
   <dimension ref="A1:H62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D27" sqref="D27"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3439,6 +3581,498 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7B41EC8-5333-4873-95EB-41672CC1E8FC}">
+  <dimension ref="A1:H19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="5.265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.19921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.86328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.59765625" customWidth="1"/>
+    <col min="5" max="5" width="35.73046875" customWidth="1"/>
+    <col min="6" max="6" width="12.19921875" style="70" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.46484375" style="70" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="29.19921875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A1" s="37" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="37" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="38" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="38" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="37" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="37" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A2" s="67">
+        <v>1</v>
+      </c>
+      <c r="B2" s="68" t="s">
+        <v>65</v>
+      </c>
+      <c r="C2" s="67" t="s">
+        <v>87</v>
+      </c>
+      <c r="D2" s="68" t="s">
+        <v>346</v>
+      </c>
+      <c r="E2" s="69" t="s">
+        <v>348</v>
+      </c>
+      <c r="F2" s="67" t="s">
+        <v>349</v>
+      </c>
+      <c r="G2" s="67" t="s">
+        <v>350</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A3" s="67">
+        <v>1</v>
+      </c>
+      <c r="B3" s="68" t="s">
+        <v>65</v>
+      </c>
+      <c r="C3" s="67" t="s">
+        <v>87</v>
+      </c>
+      <c r="D3" s="68" t="s">
+        <v>347</v>
+      </c>
+      <c r="E3" s="69" t="s">
+        <v>355</v>
+      </c>
+      <c r="F3" s="67" t="s">
+        <v>147</v>
+      </c>
+      <c r="G3" s="67" t="s">
+        <v>364</v>
+      </c>
+      <c r="H3" s="1"/>
+    </row>
+    <row r="4" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A4" s="67">
+        <v>1</v>
+      </c>
+      <c r="B4" s="68" t="s">
+        <v>65</v>
+      </c>
+      <c r="C4" s="67" t="s">
+        <v>87</v>
+      </c>
+      <c r="D4" s="68" t="s">
+        <v>347</v>
+      </c>
+      <c r="E4" s="69" t="s">
+        <v>354</v>
+      </c>
+      <c r="F4" s="70" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" s="67" t="s">
+        <v>361</v>
+      </c>
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A5" s="67">
+        <v>1</v>
+      </c>
+      <c r="B5" s="68" t="s">
+        <v>65</v>
+      </c>
+      <c r="C5" s="67" t="s">
+        <v>87</v>
+      </c>
+      <c r="D5" s="68" t="s">
+        <v>347</v>
+      </c>
+      <c r="E5" s="69" t="s">
+        <v>351</v>
+      </c>
+      <c r="F5" s="67" t="s">
+        <v>356</v>
+      </c>
+      <c r="G5" s="67" t="s">
+        <v>357</v>
+      </c>
+      <c r="H5" s="1"/>
+    </row>
+    <row r="6" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A6" s="67">
+        <v>1</v>
+      </c>
+      <c r="B6" s="68" t="s">
+        <v>65</v>
+      </c>
+      <c r="C6" s="67" t="s">
+        <v>87</v>
+      </c>
+      <c r="D6" s="68" t="s">
+        <v>347</v>
+      </c>
+      <c r="E6" s="69" t="s">
+        <v>352</v>
+      </c>
+      <c r="F6" s="67" t="s">
+        <v>147</v>
+      </c>
+      <c r="G6" s="67" t="s">
+        <v>358</v>
+      </c>
+      <c r="H6" s="1"/>
+    </row>
+    <row r="7" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A7" s="67">
+        <v>1</v>
+      </c>
+      <c r="B7" s="68" t="s">
+        <v>65</v>
+      </c>
+      <c r="C7" s="67" t="s">
+        <v>87</v>
+      </c>
+      <c r="D7" s="68" t="s">
+        <v>347</v>
+      </c>
+      <c r="E7" s="69" t="s">
+        <v>353</v>
+      </c>
+      <c r="F7" s="67" t="s">
+        <v>362</v>
+      </c>
+      <c r="G7" s="67" t="s">
+        <v>363</v>
+      </c>
+      <c r="H7" s="1"/>
+    </row>
+    <row r="8" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A8" s="67">
+        <v>1</v>
+      </c>
+      <c r="B8" s="68" t="s">
+        <v>65</v>
+      </c>
+      <c r="C8" s="67" t="s">
+        <v>87</v>
+      </c>
+      <c r="D8" s="68" t="s">
+        <v>347</v>
+      </c>
+      <c r="E8" s="69" t="s">
+        <v>359</v>
+      </c>
+      <c r="F8" s="67" t="s">
+        <v>20</v>
+      </c>
+      <c r="G8" s="67" t="s">
+        <v>360</v>
+      </c>
+      <c r="H8" s="1"/>
+    </row>
+    <row r="9" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A9" s="11">
+        <v>1</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>347</v>
+      </c>
+      <c r="E9" s="71" t="s">
+        <v>365</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>366</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>367</v>
+      </c>
+      <c r="H9" s="1"/>
+    </row>
+    <row r="10" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A10" s="67">
+        <v>1</v>
+      </c>
+      <c r="B10" s="68" t="s">
+        <v>65</v>
+      </c>
+      <c r="C10" s="67" t="s">
+        <v>87</v>
+      </c>
+      <c r="D10" s="68" t="s">
+        <v>347</v>
+      </c>
+      <c r="E10" s="69" t="s">
+        <v>359</v>
+      </c>
+      <c r="F10" s="67" t="s">
+        <v>20</v>
+      </c>
+      <c r="G10" s="67" t="s">
+        <v>360</v>
+      </c>
+      <c r="H10" s="1"/>
+    </row>
+    <row r="11" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A11" s="67">
+        <v>1</v>
+      </c>
+      <c r="B11" s="68" t="s">
+        <v>65</v>
+      </c>
+      <c r="C11" s="67" t="s">
+        <v>87</v>
+      </c>
+      <c r="D11" s="68" t="s">
+        <v>347</v>
+      </c>
+      <c r="E11" s="69" t="s">
+        <v>359</v>
+      </c>
+      <c r="F11" s="67" t="s">
+        <v>20</v>
+      </c>
+      <c r="G11" s="67" t="s">
+        <v>360</v>
+      </c>
+      <c r="H11" s="1"/>
+    </row>
+    <row r="12" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A12" s="67">
+        <v>1</v>
+      </c>
+      <c r="B12" s="68" t="s">
+        <v>368</v>
+      </c>
+      <c r="C12" s="67" t="s">
+        <v>87</v>
+      </c>
+      <c r="D12" s="68" t="s">
+        <v>346</v>
+      </c>
+      <c r="E12" s="69" t="s">
+        <v>369</v>
+      </c>
+      <c r="F12" s="67" t="s">
+        <v>370</v>
+      </c>
+      <c r="G12" s="67" t="s">
+        <v>371</v>
+      </c>
+      <c r="H12" s="1"/>
+    </row>
+    <row r="13" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A13" s="67">
+        <v>1</v>
+      </c>
+      <c r="B13" s="68" t="s">
+        <v>368</v>
+      </c>
+      <c r="C13" s="67" t="s">
+        <v>87</v>
+      </c>
+      <c r="D13" s="68" t="s">
+        <v>347</v>
+      </c>
+      <c r="E13" s="69" t="s">
+        <v>359</v>
+      </c>
+      <c r="F13" s="67" t="s">
+        <v>372</v>
+      </c>
+      <c r="G13" s="67" t="s">
+        <v>373</v>
+      </c>
+      <c r="H13" s="1"/>
+    </row>
+    <row r="14" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A14" s="67">
+        <v>1</v>
+      </c>
+      <c r="B14" s="68" t="s">
+        <v>368</v>
+      </c>
+      <c r="C14" s="67" t="s">
+        <v>87</v>
+      </c>
+      <c r="D14" s="68" t="s">
+        <v>347</v>
+      </c>
+      <c r="E14" s="69" t="s">
+        <v>374</v>
+      </c>
+      <c r="F14" s="67" t="s">
+        <v>375</v>
+      </c>
+      <c r="G14" s="67" t="s">
+        <v>376</v>
+      </c>
+      <c r="H14" s="1"/>
+    </row>
+    <row r="15" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A15" s="67">
+        <v>1</v>
+      </c>
+      <c r="B15" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="C15" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="D15" s="68" t="s">
+        <v>346</v>
+      </c>
+      <c r="E15" s="69" t="s">
+        <v>377</v>
+      </c>
+      <c r="F15" s="67" t="s">
+        <v>378</v>
+      </c>
+      <c r="G15" s="67" t="s">
+        <v>379</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A16" s="67">
+        <v>1</v>
+      </c>
+      <c r="B16" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="C16" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="D16" s="68" t="s">
+        <v>346</v>
+      </c>
+      <c r="E16" s="69" t="s">
+        <v>380</v>
+      </c>
+      <c r="F16" s="67" t="s">
+        <v>381</v>
+      </c>
+      <c r="G16" s="67" t="s">
+        <v>382</v>
+      </c>
+      <c r="H16" s="1"/>
+    </row>
+    <row r="17" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A17" s="67">
+        <v>1</v>
+      </c>
+      <c r="B17" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="C17" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="D17" s="68" t="s">
+        <v>347</v>
+      </c>
+      <c r="E17" s="69" t="s">
+        <v>383</v>
+      </c>
+      <c r="F17" s="67" t="s">
+        <v>384</v>
+      </c>
+      <c r="G17" s="67" t="s">
+        <v>385</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A18" s="67">
+        <v>1</v>
+      </c>
+      <c r="B18" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="C18" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="D18" s="68" t="s">
+        <v>347</v>
+      </c>
+      <c r="E18" s="69" t="s">
+        <v>374</v>
+      </c>
+      <c r="F18" s="67" t="s">
+        <v>386</v>
+      </c>
+      <c r="G18" s="67" t="s">
+        <v>387</v>
+      </c>
+      <c r="H18" s="1"/>
+    </row>
+    <row r="19" spans="1:8" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A19" s="11">
+        <v>1</v>
+      </c>
+      <c r="B19" s="72" t="s">
+        <v>388</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="D19" s="12" t="s">
+        <v>347</v>
+      </c>
+      <c r="E19" s="71" t="s">
+        <v>374</v>
+      </c>
+      <c r="F19" s="11" t="s">
+        <v>366</v>
+      </c>
+      <c r="G19" s="11" t="s">
+        <v>367</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>389</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6298E22-CAFA-4DDD-AF4D-CCE1042CB008}">
   <dimension ref="A1:I35"/>
   <sheetViews>
@@ -3463,14 +4097,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="F1" s="65" t="s">
+      <c r="F1" s="66" t="s">
         <v>292</v>
       </c>
-      <c r="G1" s="65"/>
-      <c r="H1" s="65" t="s">
+      <c r="G1" s="66"/>
+      <c r="H1" s="66" t="s">
         <v>291</v>
       </c>
-      <c r="I1" s="65"/>
+      <c r="I1" s="66"/>
     </row>
     <row r="2" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A2" s="7" t="s">
@@ -4396,7 +5030,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28281FF4-2F53-486B-9406-1DAD9CD507A7}">
   <sheetPr filterMode="1"/>
   <dimension ref="A1:I33"/>
@@ -5262,7 +5896,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{406A18D3-3750-49D4-BD02-AFCEEEB93861}">
   <dimension ref="A1:E19"/>
   <sheetViews>
@@ -5293,260 +5927,260 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A2" s="66" t="s">
+      <c r="A2" s="2" t="s">
         <v>325</v>
       </c>
-      <c r="B2" s="67">
+      <c r="B2" s="3">
         <v>96</v>
       </c>
-      <c r="C2" s="67" t="s">
+      <c r="C2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="67" t="s">
+      <c r="D2" s="3" t="s">
         <v>227</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A3" s="66" t="s">
+      <c r="A3" s="2" t="s">
         <v>325</v>
       </c>
-      <c r="B3" s="67">
+      <c r="B3" s="3">
         <v>10</v>
       </c>
-      <c r="C3" s="67" t="s">
+      <c r="C3" s="3" t="s">
         <v>327</v>
       </c>
-      <c r="D3" s="67" t="s">
+      <c r="D3" s="3" t="s">
         <v>328</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A4" s="66" t="s">
+      <c r="A4" s="2" t="s">
         <v>325</v>
       </c>
-      <c r="B4" s="67">
+      <c r="B4" s="3">
         <v>20</v>
       </c>
-      <c r="C4" s="67" t="s">
+      <c r="C4" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="D4" s="67" t="s">
+      <c r="D4" s="3" t="s">
         <v>326</v>
       </c>
-      <c r="E4" s="72" t="s">
+      <c r="E4" s="65" t="s">
         <v>338</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A5" s="66" t="s">
+      <c r="A5" s="2" t="s">
         <v>325</v>
       </c>
-      <c r="B5" s="67">
+      <c r="B5" s="3">
         <v>30</v>
       </c>
-      <c r="C5" s="67" t="s">
+      <c r="C5" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="67" t="s">
+      <c r="D5" s="3" t="s">
         <v>329</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A6" s="66" t="s">
+      <c r="A6" s="2" t="s">
         <v>325</v>
       </c>
-      <c r="B6" s="67">
+      <c r="B6" s="3">
         <v>40</v>
       </c>
-      <c r="C6" s="67" t="s">
+      <c r="C6" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="67" t="s">
+      <c r="D6" s="3" t="s">
         <v>330</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="28.9" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A7" s="70" t="s">
+      <c r="A7" s="8" t="s">
         <v>325</v>
       </c>
-      <c r="B7" s="71">
+      <c r="B7" s="9">
         <v>50</v>
       </c>
-      <c r="C7" s="71" t="s">
+      <c r="C7" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="71" t="s">
+      <c r="D7" s="9" t="s">
         <v>331</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A8" s="68" t="s">
+      <c r="A8" s="21" t="s">
         <v>332</v>
       </c>
-      <c r="B8" s="69">
+      <c r="B8" s="20">
         <v>96</v>
       </c>
-      <c r="C8" s="69" t="s">
+      <c r="C8" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="69" t="s">
+      <c r="D8" s="20" t="s">
         <v>273</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A9" s="68" t="s">
+      <c r="A9" s="21" t="s">
         <v>332</v>
       </c>
-      <c r="B9" s="69">
+      <c r="B9" s="20">
         <v>10</v>
       </c>
-      <c r="C9" s="69" t="s">
+      <c r="C9" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="69" t="s">
+      <c r="D9" s="20" t="s">
         <v>333</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A10" s="68" t="s">
+      <c r="A10" s="21" t="s">
         <v>332</v>
       </c>
-      <c r="B10" s="69">
+      <c r="B10" s="20">
         <v>20</v>
       </c>
-      <c r="C10" s="69" t="s">
+      <c r="C10" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="69" t="s">
+      <c r="D10" s="20" t="s">
         <v>334</v>
       </c>
-      <c r="E10" s="72" t="s">
+      <c r="E10" s="65" t="s">
         <v>338</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A11" s="68" t="s">
+      <c r="A11" s="21" t="s">
         <v>332</v>
       </c>
-      <c r="B11" s="69">
+      <c r="B11" s="20">
         <v>30</v>
       </c>
-      <c r="C11" s="69" t="s">
+      <c r="C11" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="69" t="s">
+      <c r="D11" s="20" t="s">
         <v>335</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A12" s="68" t="s">
+      <c r="A12" s="21" t="s">
         <v>332</v>
       </c>
-      <c r="B12" s="69">
+      <c r="B12" s="20">
         <v>40</v>
       </c>
-      <c r="C12" s="69" t="s">
+      <c r="C12" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="D12" s="69" t="s">
+      <c r="D12" s="20" t="s">
         <v>336</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="28.9" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A13" s="70" t="s">
+      <c r="A13" s="8" t="s">
         <v>332</v>
       </c>
-      <c r="B13" s="71">
+      <c r="B13" s="9">
         <v>50</v>
       </c>
-      <c r="C13" s="71" t="s">
+      <c r="C13" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="D13" s="71" t="s">
+      <c r="D13" s="9" t="s">
         <v>337</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A14" s="68" t="s">
+      <c r="A14" s="21" t="s">
         <v>339</v>
       </c>
-      <c r="B14" s="69">
+      <c r="B14" s="20">
         <v>96</v>
       </c>
-      <c r="C14" s="69" t="s">
+      <c r="C14" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="D14" s="69" t="s">
+      <c r="D14" s="20" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A15" s="68" t="s">
+      <c r="A15" s="21" t="s">
         <v>339</v>
       </c>
-      <c r="B15" s="69">
+      <c r="B15" s="20">
         <v>10</v>
       </c>
-      <c r="C15" s="69" t="s">
+      <c r="C15" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="D15" s="69" t="s">
+      <c r="D15" s="20" t="s">
         <v>340</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A16" s="68" t="s">
+      <c r="A16" s="21" t="s">
         <v>339</v>
       </c>
-      <c r="B16" s="69">
+      <c r="B16" s="20">
         <v>20</v>
       </c>
-      <c r="C16" s="69" t="s">
+      <c r="C16" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="D16" s="69" t="s">
+      <c r="D16" s="20" t="s">
         <v>341</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A17" s="68" t="s">
+      <c r="A17" s="21" t="s">
         <v>339</v>
       </c>
-      <c r="B17" s="69">
+      <c r="B17" s="20">
         <v>30</v>
       </c>
-      <c r="C17" s="69" t="s">
+      <c r="C17" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="D17" s="69" t="s">
+      <c r="D17" s="20" t="s">
         <v>342</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A18" s="68" t="s">
+      <c r="A18" s="21" t="s">
         <v>339</v>
       </c>
-      <c r="B18" s="69">
+      <c r="B18" s="20">
         <v>40</v>
       </c>
-      <c r="C18" s="69" t="s">
+      <c r="C18" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="D18" s="69" t="s">
+      <c r="D18" s="20" t="s">
         <v>343</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A19" s="68" t="s">
+      <c r="A19" s="21" t="s">
         <v>339</v>
       </c>
-      <c r="B19" s="69">
+      <c r="B19" s="20">
         <v>50</v>
       </c>
-      <c r="C19" s="69" t="s">
+      <c r="C19" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="D19" s="69" t="s">
+      <c r="D19" s="20" t="s">
         <v>344</v>
       </c>
     </row>

</xml_diff>